<commit_message>
Backup QR Scanner data - 2025-12-29T09:10:29.461Z - Cache Bust: 1766999429461
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1902,9 +1902,69 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>201888</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C76" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D76" t="str">
+        <v>11:00:55</v>
+      </c>
+      <c r="E76" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F76" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>201243</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C77" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D77" t="str">
+        <v>11:06:16</v>
+      </c>
+      <c r="E77" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F77" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>201479</v>
+      </c>
+      <c r="B78" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C78" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D78" t="str">
+        <v>11:10:24</v>
+      </c>
+      <c r="E78" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F78" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F75"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F78"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-12-29T09:10:37.174Z - Cache Bust ID: 1766999437174s59b1urhe
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1902,69 +1902,9 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="str">
-        <v>201888</v>
-      </c>
-      <c r="B76" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C76" t="str">
-        <v>29/12/2025</v>
-      </c>
-      <c r="D76" t="str">
-        <v>11:00:55</v>
-      </c>
-      <c r="E76" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F76" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="str">
-        <v>201243</v>
-      </c>
-      <c r="B77" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C77" t="str">
-        <v>29/12/2025</v>
-      </c>
-      <c r="D77" t="str">
-        <v>11:06:16</v>
-      </c>
-      <c r="E77" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F77" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="str">
-        <v>201479</v>
-      </c>
-      <c r="B78" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C78" t="str">
-        <v>29/12/2025</v>
-      </c>
-      <c r="D78" t="str">
-        <v>11:10:24</v>
-      </c>
-      <c r="E78" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F78" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F78"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F75"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-12-29T11:41:54.153Z - Cache Bust: 1767008514153
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1902,9 +1902,209 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>201888</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C76" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D76" t="str">
+        <v>11:00:55</v>
+      </c>
+      <c r="E76" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F76" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>201243</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C77" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D77" t="str">
+        <v>11:06:16</v>
+      </c>
+      <c r="E77" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F77" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>201479</v>
+      </c>
+      <c r="B78" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C78" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D78" t="str">
+        <v>11:10:24</v>
+      </c>
+      <c r="E78" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F78" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>201322</v>
+      </c>
+      <c r="B79" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C79" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D79" t="str">
+        <v>13:39:28</v>
+      </c>
+      <c r="E79" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F79" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>201265</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C80" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D80" t="str">
+        <v>13:39:32</v>
+      </c>
+      <c r="E80" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F80" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>201234</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C81" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D81" t="str">
+        <v>13:39:37</v>
+      </c>
+      <c r="E81" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F81" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>201329</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C82" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D82" t="str">
+        <v>13:39:39</v>
+      </c>
+      <c r="E82" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F82" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>201239</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C83" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D83" t="str">
+        <v>13:39:45</v>
+      </c>
+      <c r="E83" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F83" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>201061</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C84" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D84" t="str">
+        <v>13:40:04</v>
+      </c>
+      <c r="E84" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F84" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>201416</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C85" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D85" t="str">
+        <v>13:40:09</v>
+      </c>
+      <c r="E85" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F85" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F75"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F85"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-12-29T11:57:03.079Z - Cache Bust: 1767009423079
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2102,9 +2102,29 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>201560</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C86" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D86" t="str">
+        <v>13:57:00</v>
+      </c>
+      <c r="E86" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F86" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F85"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F86"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edited session - 2025-12-29T11:57:19.967Z - Cache Bust ID: 1767009439967vumw481ck
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Neurology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2102,29 +2102,9 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" t="str">
-        <v>201560</v>
-      </c>
-      <c r="B86" t="str">
-        <v>Neurology</v>
-      </c>
-      <c r="C86" t="str">
-        <v>29/12/2025</v>
-      </c>
-      <c r="D86" t="str">
-        <v>13:57:00</v>
-      </c>
-      <c r="E86" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F86" t="str">
-        <v>emp17.farah.a.youssef@gmail.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F86"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F85"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2026-01-17T08:40:27.053Z - Cache Bust: 1768639227053
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
+++ b/log_history/Y5_B2526_Neurology_scanner1766998399527_b4df4d3060ee5a11a9fb4fe245eb3c4dfaf42a930352ff25ac8e7238642d95b9.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2102,9 +2102,29 @@
         <v>emp17.farah.a.youssef@gmail.com</v>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>201560</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Neurology</v>
+      </c>
+      <c r="C86" t="str">
+        <v>29/12/2025</v>
+      </c>
+      <c r="D86" t="str">
+        <v>13:57:00</v>
+      </c>
+      <c r="E86" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F86" t="str">
+        <v>emp17.farah.a.youssef@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F85"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F86"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>